<commit_message>
WBS & ERD updated
</commit_message>
<xml_diff>
--- a/화면 구성/RS_유한솔_2020-08-27_v1.0.3.xlsx
+++ b/화면 구성/RS_유한솔_2020-08-27_v1.0.3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="324" yWindow="516" windowWidth="14400" windowHeight="8868"/>
+    <workbookView xWindow="320" yWindow="520" windowWidth="14400" windowHeight="8870"/>
   </bookViews>
   <sheets>
     <sheet name="시트1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
   <si>
     <t>구분</t>
   </si>
@@ -1363,6 +1363,9 @@
   </si>
   <si>
     <r>
+      <t>입력받은 내용으로 사용자의</t>
+    </r>
+    <r>
       <rPr>
         <b/>
         <sz val="11"/>
@@ -1371,6 +1374,575 @@
         <family val="3"/>
         <charset val="129"/>
       </rPr>
+      <t xml:space="preserve"> [이름], [닉네임], [소개글],[전화번호],[성별],[나이],[계열사]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> 을 수정 한다.</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>자신이 작성한 게시물의 수를 조회한다.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>case06</t>
+  </si>
+  <si>
+    <t>case11</t>
+  </si>
+  <si>
+    <t>비고</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>사용자</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>인증</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>및</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>권한에</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>따른</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>화면</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>접근제어</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>계열사</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>조회</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>전체 계열사를 조회한다.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>전체 사용자를 조회한다.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>사용자</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>차단</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">계열사의 권한을 넘어서 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>[사용자]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> 권한을 가진 사람의 기능을 차단할 수 있다.</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>공통</t>
+  </si>
+  <si>
+    <t>case01</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>case02</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>case03</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>case04</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>case05</t>
+  </si>
+  <si>
+    <t>case07</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>case08</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>Spring Scurity</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>를</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>통해</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>사용자의</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>인증</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>및</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>권한에</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>따라</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>페이지의</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>접근을</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>제어한다</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>사용자 관리</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>case09</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>case10</t>
+  </si>
+  <si>
+    <t>case12</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>case13</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>case14</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>case15</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>case16</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>case17</t>
+  </si>
+  <si>
+    <t>case18</t>
+  </si>
+  <si>
+    <t>case19</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>case20</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>case21</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>case22</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>사용자</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>차단</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">계열사의 권한을 넘어서 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>[사용자],[관리자]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> 권한을 가진 사람의 기능을 차단할 수 있다.</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
       <t>[아이디]</t>
     </r>
     <r>
@@ -1392,7 +1964,7 @@
         <family val="3"/>
         <charset val="129"/>
       </rPr>
-      <t xml:space="preserve"> [비밀번호],[이름], [성별], [나이],[전화번호],[그룹]</t>
+      <t xml:space="preserve"> [비밀번호],[이름], [성별], [나이],[전화번호],[계열사]</t>
     </r>
     <r>
       <rPr>
@@ -1403,511 +1975,6 @@
         <charset val="129"/>
       </rPr>
       <t>을 등록한다.</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>입력받은 내용으로 사용자의</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve"> [이름], [닉네임], [소개글],[전화번호],[성별],[나이],[계열사]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve"> 을 수정 한다.</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>자신이 작성한 게시물의 수를 조회한다.</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>case06</t>
-  </si>
-  <si>
-    <t>case10</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>case11</t>
-  </si>
-  <si>
-    <t>case12</t>
-  </si>
-  <si>
-    <t>case13</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>case15</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>case16</t>
-  </si>
-  <si>
-    <t>case17</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>case18</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>case20</t>
-  </si>
-  <si>
-    <t>비고</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>사용자</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>인증</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>및</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>권한에</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>따른</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>화면</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>접근제어</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>case14</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>계열사</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>조회</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>전체 계열사를 조회한다.</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>전체 사용자를 조회한다.</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>case19</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>case21</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>사용자</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>차단</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">계열사의 권한을 넘어서 </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>[사용자]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve"> 권한을 가진 사람의 기능을 차단할 수 있다.</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>공통</t>
-  </si>
-  <si>
-    <t>case09</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>case01</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>case02</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>case03</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>case04</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>case05</t>
-  </si>
-  <si>
-    <t>case07</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>case08</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>Spring Scurity</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>를</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>통해</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>사용자의</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>인증</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>및</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>권한에</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>따라</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>페이지의</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>접근을</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>제어한다</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
     </r>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -1916,7 +1983,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2022,6 +2089,19 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="돋움"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -2037,7 +2117,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="61">
+  <borders count="65">
     <border>
       <left/>
       <right/>
@@ -2779,11 +2859,53 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="127">
+  <cellXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -2793,6 +2915,81 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -2805,30 +3002,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2859,38 +3032,26 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2910,21 +3071,12 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -2973,6 +3125,18 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3000,13 +3164,16 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3014,18 +3181,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3062,18 +3217,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -3092,6 +3235,12 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3104,12 +3253,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3122,9 +3265,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3137,16 +3277,16 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3169,13 +3309,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>155090</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>61</xdr:row>
       <xdr:rowOff>138505</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>579323</xdr:colOff>
-      <xdr:row>88</xdr:row>
+      <xdr:row>90</xdr:row>
       <xdr:rowOff>60106</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3207,13 +3347,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>233530</xdr:colOff>
-      <xdr:row>91</xdr:row>
+      <xdr:row>93</xdr:row>
       <xdr:rowOff>93682</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>680625</xdr:colOff>
-      <xdr:row>120</xdr:row>
+      <xdr:row>122</xdr:row>
       <xdr:rowOff>51591</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3245,13 +3385,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1893793</xdr:colOff>
-      <xdr:row>91</xdr:row>
+      <xdr:row>93</xdr:row>
       <xdr:rowOff>77098</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>231496</xdr:colOff>
-      <xdr:row>120</xdr:row>
+      <xdr:row>122</xdr:row>
       <xdr:rowOff>42628</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3283,13 +3423,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>251460</xdr:colOff>
-      <xdr:row>122</xdr:row>
+      <xdr:row>124</xdr:row>
       <xdr:rowOff>123264</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>713796</xdr:colOff>
-      <xdr:row>151</xdr:row>
+      <xdr:row>153</xdr:row>
       <xdr:rowOff>119275</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3321,13 +3461,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>882127</xdr:colOff>
-      <xdr:row>156</xdr:row>
+      <xdr:row>158</xdr:row>
       <xdr:rowOff>190052</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>210430</xdr:colOff>
-      <xdr:row>185</xdr:row>
+      <xdr:row>187</xdr:row>
       <xdr:rowOff>147962</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3359,13 +3499,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>157</xdr:row>
+      <xdr:row>159</xdr:row>
       <xdr:rowOff>1792</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>462336</xdr:colOff>
-      <xdr:row>185</xdr:row>
+      <xdr:row>187</xdr:row>
       <xdr:rowOff>165443</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3597,40 +3737,40 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:K56"/>
+  <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.5546875" customWidth="1"/>
-    <col min="3" max="3" width="34.33203125" customWidth="1"/>
-    <col min="4" max="4" width="37.88671875" customWidth="1"/>
-    <col min="5" max="5" width="76.77734375" customWidth="1"/>
+    <col min="2" max="2" width="16.54296875" customWidth="1"/>
+    <col min="3" max="3" width="34.36328125" customWidth="1"/>
+    <col min="4" max="4" width="37.90625" customWidth="1"/>
+    <col min="5" max="5" width="76.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1" s="91" t="s">
+    <row r="1" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="102" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="93" t="s">
+      <c r="B1" s="104" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="110" t="s">
+      <c r="C1" s="119" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="93" t="s">
+      <c r="D1" s="104" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="93" t="s">
+      <c r="E1" s="104" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="95" t="s">
-        <v>65</v>
-      </c>
-      <c r="G1" s="93" t="s">
+      <c r="F1" s="106" t="s">
+        <v>56</v>
+      </c>
+      <c r="G1" s="104" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="1"/>
@@ -3638,37 +3778,37 @@
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:11" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="92"/>
-      <c r="B2" s="94"/>
-      <c r="C2" s="111"/>
-      <c r="D2" s="94"/>
-      <c r="E2" s="94"/>
-      <c r="F2" s="94"/>
-      <c r="G2" s="94"/>
+    <row r="2" spans="1:11" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="103"/>
+      <c r="B2" s="105"/>
+      <c r="C2" s="120"/>
+      <c r="D2" s="105"/>
+      <c r="E2" s="105"/>
+      <c r="F2" s="105"/>
+      <c r="G2" s="105"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="B3" s="87" t="s">
+    <row r="3" spans="1:11" ht="16.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="98" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="D3" s="85" t="s">
+      <c r="C3" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="96" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="89" t="s">
-        <v>52</v>
-      </c>
-      <c r="F3" s="77"/>
-      <c r="G3" s="79">
+      <c r="E3" s="100" t="s">
+        <v>88</v>
+      </c>
+      <c r="F3" s="40"/>
+      <c r="G3" s="94">
         <v>1</v>
       </c>
       <c r="H3" s="1"/>
@@ -3677,34 +3817,34 @@
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="9"/>
-      <c r="B4" s="88"/>
-      <c r="C4" s="68"/>
-      <c r="D4" s="86"/>
-      <c r="E4" s="90"/>
-      <c r="F4" s="123"/>
-      <c r="G4" s="124"/>
+      <c r="A4" s="34"/>
+      <c r="B4" s="99"/>
+      <c r="C4" s="82"/>
+      <c r="D4" s="97"/>
+      <c r="E4" s="101"/>
+      <c r="F4" s="129"/>
+      <c r="G4" s="130"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:11" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
-      <c r="B5" s="14" t="s">
+    <row r="5" spans="1:11" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="34"/>
+      <c r="B5" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="D5" s="81" t="s">
+      <c r="C5" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" s="115" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="81" t="s">
+      <c r="E5" s="115" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="125"/>
-      <c r="G5" s="79">
+      <c r="F5" s="131"/>
+      <c r="G5" s="94">
         <v>1</v>
       </c>
       <c r="H5" s="1"/>
@@ -3713,34 +3853,34 @@
       <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:11" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="9"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="68"/>
-      <c r="D6" s="82"/>
-      <c r="E6" s="82"/>
-      <c r="F6" s="126"/>
-      <c r="G6" s="124"/>
+      <c r="A6" s="34"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="82"/>
+      <c r="D6" s="116"/>
+      <c r="E6" s="116"/>
+      <c r="F6" s="132"/>
+      <c r="G6" s="130"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-      <c r="B7" s="14" t="s">
+      <c r="A7" s="34"/>
+      <c r="B7" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="D7" s="83" t="s">
+      <c r="C7" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="112" t="s">
+      <c r="E7" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="F7" s="77"/>
-      <c r="G7" s="79">
+      <c r="F7" s="40"/>
+      <c r="G7" s="94">
         <v>2</v>
       </c>
       <c r="H7" s="1"/>
@@ -3748,33 +3888,33 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="84"/>
-      <c r="E8" s="113"/>
-      <c r="F8" s="78"/>
-      <c r="G8" s="80"/>
+    <row r="8" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="34"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="91"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="93"/>
+      <c r="G8" s="95"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
     </row>
     <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="D9" s="69" t="s">
+      <c r="A9" s="34"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" s="83" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="114" t="s">
-        <v>53</v>
-      </c>
-      <c r="F9" s="46"/>
-      <c r="G9" s="50">
+      <c r="E9" s="121" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="13"/>
+      <c r="G9" s="15">
         <v>1</v>
       </c>
       <c r="H9" s="1"/>
@@ -3783,31 +3923,31 @@
       <c r="K9" s="1"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="70"/>
-      <c r="E10" s="115"/>
-      <c r="F10" s="47"/>
-      <c r="G10" s="35"/>
+      <c r="A10" s="34"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="84"/>
+      <c r="E10" s="122"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="16"/>
       <c r="I10" s="2"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
     </row>
     <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="29" t="s">
-        <v>81</v>
-      </c>
-      <c r="D11" s="69" t="s">
+      <c r="A11" s="34"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" s="83" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="74" t="s">
-        <v>54</v>
-      </c>
-      <c r="F11" s="46"/>
-      <c r="G11" s="50">
+      <c r="E11" s="88" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="13"/>
+      <c r="G11" s="15">
         <v>1</v>
       </c>
       <c r="H11" s="1"/>
@@ -3816,32 +3956,32 @@
       <c r="K11" s="1"/>
     </row>
     <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="70"/>
-      <c r="E12" s="75"/>
-      <c r="F12" s="47"/>
-      <c r="G12" s="35"/>
+      <c r="A12" s="34"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="84"/>
+      <c r="E12" s="89"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="16"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
     </row>
     <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="29" t="s">
-        <v>55</v>
-      </c>
-      <c r="D13" s="69" t="s">
+      <c r="A13" s="34"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="83" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="74" t="s">
+      <c r="E13" s="88" t="s">
         <v>39</v>
       </c>
-      <c r="F13" s="46"/>
-      <c r="G13" s="50">
+      <c r="F13" s="13"/>
+      <c r="G13" s="15">
         <v>1</v>
       </c>
       <c r="H13" s="1"/>
@@ -3850,32 +3990,32 @@
       <c r="K13" s="1"/>
     </row>
     <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="70"/>
-      <c r="E14" s="75"/>
-      <c r="F14" s="47"/>
-      <c r="G14" s="35"/>
+      <c r="A14" s="34"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="84"/>
+      <c r="E14" s="89"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="16"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="D15" s="69" t="s">
+    <row r="15" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="34"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15" s="83" t="s">
         <v>20</v>
       </c>
-      <c r="E15" s="74" t="s">
+      <c r="E15" s="88" t="s">
         <v>40</v>
       </c>
-      <c r="F15" s="46"/>
-      <c r="G15" s="50">
+      <c r="F15" s="13"/>
+      <c r="G15" s="15">
         <v>1</v>
       </c>
       <c r="H15" s="1"/>
@@ -3883,35 +4023,35 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:11" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="9"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="68"/>
-      <c r="D16" s="71"/>
-      <c r="E16" s="116"/>
-      <c r="F16" s="76"/>
-      <c r="G16" s="51"/>
+    <row r="16" spans="1:11" ht="13.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="34"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="82"/>
+      <c r="D16" s="85"/>
+      <c r="E16" s="123"/>
+      <c r="F16" s="92"/>
+      <c r="G16" s="61"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="1:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
-      <c r="B17" s="14" t="s">
+    <row r="17" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="34"/>
+      <c r="B17" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="D17" s="108" t="s">
+      <c r="C17" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" s="117" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="117" t="s">
+      <c r="E17" s="124" t="s">
         <v>43</v>
       </c>
-      <c r="F17" s="67"/>
-      <c r="G17" s="34">
+      <c r="F17" s="81"/>
+      <c r="G17" s="46">
         <v>1</v>
       </c>
       <c r="H17" s="1"/>
@@ -3919,61 +4059,61 @@
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="70"/>
-      <c r="E18" s="115"/>
-      <c r="F18" s="47"/>
-      <c r="G18" s="35"/>
+    <row r="18" spans="1:11" ht="15.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="34"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="84"/>
+      <c r="E18" s="122"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="16"/>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="9"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="29" t="s">
-        <v>56</v>
-      </c>
-      <c r="D19" s="69" t="s">
+    <row r="19" spans="1:11" ht="15.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="34"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" s="83" t="s">
         <v>30</v>
       </c>
-      <c r="E19" s="74" t="s">
+      <c r="E19" s="88" t="s">
         <v>29</v>
       </c>
-      <c r="F19" s="46"/>
-      <c r="G19" s="50" t="s">
+      <c r="F19" s="13"/>
+      <c r="G19" s="15" t="s">
         <v>17</v>
       </c>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="1:11" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="9"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="70"/>
-      <c r="E20" s="75"/>
-      <c r="F20" s="47"/>
-      <c r="G20" s="35"/>
+    <row r="20" spans="1:11" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="34"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="84"/>
+      <c r="E20" s="89"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="16"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
     </row>
-    <row r="21" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="9"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="29" t="s">
-        <v>57</v>
-      </c>
-      <c r="D21" s="104" t="s">
+    <row r="21" spans="1:11" ht="15.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="34"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D21" s="111" t="s">
         <v>13</v>
       </c>
-      <c r="E21" s="102" t="s">
+      <c r="E21" s="109" t="s">
         <v>47</v>
       </c>
-      <c r="F21" s="48"/>
-      <c r="G21" s="50">
+      <c r="F21" s="59"/>
+      <c r="G21" s="15">
         <v>1</v>
       </c>
       <c r="H21" s="1"/>
@@ -3981,33 +4121,33 @@
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
     </row>
-    <row r="22" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="9"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="105"/>
-      <c r="E22" s="103"/>
-      <c r="F22" s="62"/>
-      <c r="G22" s="35"/>
+    <row r="22" spans="1:11" ht="15.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="34"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="112"/>
+      <c r="E22" s="110"/>
+      <c r="F22" s="72"/>
+      <c r="G22" s="16"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
     </row>
-    <row r="23" spans="1:11" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="9"/>
-      <c r="B23" s="15"/>
-      <c r="C23" s="29" t="s">
-        <v>58</v>
-      </c>
-      <c r="D23" s="104" t="s">
+    <row r="23" spans="1:11" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="34"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23" s="111" t="s">
         <v>14</v>
       </c>
-      <c r="E23" s="102" t="s">
+      <c r="E23" s="109" t="s">
         <v>41</v>
       </c>
-      <c r="F23" s="48"/>
-      <c r="G23" s="50">
+      <c r="F23" s="59"/>
+      <c r="G23" s="15">
         <v>1</v>
       </c>
       <c r="H23" s="1"/>
@@ -4015,33 +4155,33 @@
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
     </row>
-    <row r="24" spans="1:11" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="9"/>
-      <c r="B24" s="15"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="105"/>
-      <c r="E24" s="103"/>
-      <c r="F24" s="62"/>
-      <c r="G24" s="35"/>
+    <row r="24" spans="1:11" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="34"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="112"/>
+      <c r="E24" s="110"/>
+      <c r="F24" s="72"/>
+      <c r="G24" s="16"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
     </row>
-    <row r="25" spans="1:11" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="9"/>
-      <c r="B25" s="15"/>
-      <c r="C25" s="29" t="s">
-        <v>59</v>
-      </c>
-      <c r="D25" s="69" t="s">
+    <row r="25" spans="1:11" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="34"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D25" s="83" t="s">
         <v>15</v>
       </c>
-      <c r="E25" s="72" t="s">
+      <c r="E25" s="86" t="s">
         <v>42</v>
       </c>
-      <c r="F25" s="48"/>
-      <c r="G25" s="50">
+      <c r="F25" s="59"/>
+      <c r="G25" s="15">
         <v>1</v>
       </c>
       <c r="H25" s="1"/>
@@ -4049,289 +4189,323 @@
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
     </row>
-    <row r="26" spans="1:11" ht="13.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="10"/>
-      <c r="B26" s="16"/>
-      <c r="C26" s="68"/>
-      <c r="D26" s="71"/>
-      <c r="E26" s="73"/>
-      <c r="F26" s="49"/>
-      <c r="G26" s="51"/>
+    <row r="26" spans="1:11" ht="13.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="35"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="82"/>
+      <c r="D26" s="85"/>
+      <c r="E26" s="87"/>
+      <c r="F26" s="60"/>
+      <c r="G26" s="61"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
     </row>
-    <row r="27" spans="1:11" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="11" t="s">
+    <row r="27" spans="1:11" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="C27" s="17" t="s">
+      <c r="B27" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="C27" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="D27" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="E27" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="F27" s="23"/>
-      <c r="G27" s="7">
-        <v>1</v>
-      </c>
+      <c r="D27" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="E27" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="F27" s="28"/>
+      <c r="G27" s="30"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
-    </row>
-    <row r="28" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="12"/>
-      <c r="B28" s="15"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="8"/>
+      <c r="K27" s="1"/>
+    </row>
+    <row r="28" spans="1:11" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="21"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="31"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
-    </row>
-    <row r="29" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="12"/>
-      <c r="B29" s="15"/>
-      <c r="C29" s="118" t="s">
-        <v>67</v>
-      </c>
-      <c r="D29" s="119" t="s">
-        <v>68</v>
-      </c>
-      <c r="E29" s="121" t="s">
-        <v>69</v>
-      </c>
-      <c r="F29" s="61"/>
-      <c r="G29" s="52">
+      <c r="K28" s="1"/>
+    </row>
+    <row r="29" spans="1:11" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="21"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="F29" s="13"/>
+      <c r="G29" s="15">
         <v>1</v>
       </c>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
-    </row>
-    <row r="30" spans="1:11" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="12"/>
-      <c r="B30" s="15"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="120"/>
-      <c r="E30" s="122"/>
-      <c r="F30" s="109"/>
-      <c r="G30" s="53"/>
+      <c r="K29" s="1"/>
+    </row>
+    <row r="30" spans="1:11" ht="13.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="21"/>
+      <c r="B30" s="19"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="16"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
-    </row>
-    <row r="31" spans="1:11" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="12"/>
-      <c r="B31" s="15"/>
-      <c r="C31" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="D31" s="42" t="s">
-        <v>36</v>
-      </c>
-      <c r="E31" s="56" t="s">
-        <v>44</v>
-      </c>
-      <c r="F31" s="61"/>
-      <c r="G31" s="52">
+      <c r="K30" s="1"/>
+    </row>
+    <row r="31" spans="1:11" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="21"/>
+      <c r="B31" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C31" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="D31" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="E31" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="F31" s="40"/>
+      <c r="G31" s="32">
         <v>1</v>
       </c>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
     </row>
-    <row r="32" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="12"/>
-      <c r="B32" s="15"/>
-      <c r="C32" s="40"/>
-      <c r="D32" s="43"/>
-      <c r="E32" s="57"/>
-      <c r="F32" s="62"/>
-      <c r="G32" s="35"/>
-    </row>
-    <row r="33" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="12"/>
-      <c r="B33" s="15"/>
-      <c r="C33" s="18" t="s">
+    <row r="32" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="21"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="37"/>
+      <c r="E32" s="39"/>
+      <c r="F32" s="41"/>
+      <c r="G32" s="33"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+    </row>
+    <row r="33" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="21"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="52" t="s">
+        <v>79</v>
+      </c>
+      <c r="D33" s="125" t="s">
+        <v>58</v>
+      </c>
+      <c r="E33" s="127" t="s">
+        <v>59</v>
+      </c>
+      <c r="F33" s="71"/>
+      <c r="G33" s="62">
+        <v>1</v>
+      </c>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+    </row>
+    <row r="34" spans="1:10" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="21"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="126"/>
+      <c r="E34" s="128"/>
+      <c r="F34" s="118"/>
+      <c r="G34" s="63"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+    </row>
+    <row r="35" spans="1:10" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="21"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="52" t="s">
+        <v>80</v>
+      </c>
+      <c r="D35" s="55" t="s">
+        <v>36</v>
+      </c>
+      <c r="E35" s="66" t="s">
+        <v>44</v>
+      </c>
+      <c r="F35" s="71"/>
+      <c r="G35" s="62">
+        <v>1</v>
+      </c>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+    </row>
+    <row r="36" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="21"/>
+      <c r="B36" s="18"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="56"/>
+      <c r="E36" s="67"/>
+      <c r="F36" s="72"/>
+      <c r="G36" s="16"/>
+    </row>
+    <row r="37" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="21"/>
+      <c r="B37" s="18"/>
+      <c r="C37" s="52" t="s">
+        <v>81</v>
+      </c>
+      <c r="D37" s="57" t="s">
+        <v>37</v>
+      </c>
+      <c r="E37" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F37" s="73"/>
+      <c r="G37" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="21"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="58"/>
+      <c r="E38" s="68"/>
+      <c r="F38" s="74"/>
+      <c r="G38" s="63"/>
+    </row>
+    <row r="39" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="21"/>
+      <c r="B39" s="18"/>
+      <c r="C39" s="53" t="s">
+        <v>82</v>
+      </c>
+      <c r="D39" s="64" t="s">
+        <v>38</v>
+      </c>
+      <c r="E39" s="69" t="s">
+        <v>46</v>
+      </c>
+      <c r="F39" s="75"/>
+      <c r="G39" s="62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="22"/>
+      <c r="B40" s="19"/>
+      <c r="C40" s="54"/>
+      <c r="D40" s="65"/>
+      <c r="E40" s="70"/>
+      <c r="F40" s="76"/>
+      <c r="G40" s="61"/>
+    </row>
+    <row r="41" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="45" t="s">
+        <v>26</v>
+      </c>
+      <c r="B41" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="C41" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="D41" s="50" t="s">
+        <v>33</v>
+      </c>
+      <c r="E41" s="49" t="s">
+        <v>60</v>
+      </c>
+      <c r="F41" s="47"/>
+      <c r="G41" s="46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="34"/>
+      <c r="B42" s="43"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="51"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="48"/>
+      <c r="G42" s="16"/>
+    </row>
+    <row r="43" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="34"/>
+      <c r="B43" s="43"/>
+      <c r="C43" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D43" s="113" t="s">
+        <v>24</v>
+      </c>
+      <c r="E43" s="107" t="s">
+        <v>51</v>
+      </c>
+      <c r="F43" s="13"/>
+      <c r="G43" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="34"/>
+      <c r="B44" s="43"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="114"/>
+      <c r="E44" s="108"/>
+      <c r="F44" s="14"/>
+      <c r="G44" s="16"/>
+    </row>
+    <row r="45" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="34"/>
+      <c r="B45" s="43"/>
+      <c r="C45" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D45" s="77" t="s">
         <v>61</v>
       </c>
-      <c r="D33" s="44" t="s">
-        <v>37</v>
-      </c>
-      <c r="E33" s="32" t="s">
-        <v>45</v>
-      </c>
-      <c r="F33" s="63"/>
-      <c r="G33" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="12"/>
-      <c r="B34" s="15"/>
-      <c r="C34" s="40"/>
-      <c r="D34" s="45"/>
-      <c r="E34" s="58"/>
-      <c r="F34" s="64"/>
-      <c r="G34" s="53"/>
-    </row>
-    <row r="35" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="12"/>
-      <c r="B35" s="15"/>
-      <c r="C35" s="40" t="s">
+      <c r="E45" s="79" t="s">
         <v>62</v>
       </c>
-      <c r="D35" s="54" t="s">
-        <v>38</v>
-      </c>
-      <c r="E35" s="59" t="s">
-        <v>46</v>
-      </c>
-      <c r="F35" s="65"/>
-      <c r="G35" s="52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="13"/>
-      <c r="B36" s="16"/>
-      <c r="C36" s="41"/>
-      <c r="D36" s="55"/>
-      <c r="E36" s="60"/>
-      <c r="F36" s="66"/>
-      <c r="G36" s="51"/>
-    </row>
-    <row r="37" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="B37" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="C37" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="D37" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="E37" s="38" t="s">
-        <v>70</v>
-      </c>
-      <c r="F37" s="36"/>
-      <c r="G37" s="34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="9"/>
-      <c r="B38" s="26"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="31"/>
-      <c r="E38" s="33"/>
-      <c r="F38" s="37"/>
-      <c r="G38" s="35"/>
-    </row>
-    <row r="39" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="9"/>
-      <c r="B39" s="26"/>
-      <c r="C39" s="29" t="s">
-        <v>71</v>
-      </c>
-      <c r="D39" s="106" t="s">
-        <v>24</v>
-      </c>
-      <c r="E39" s="96" t="s">
-        <v>51</v>
-      </c>
-      <c r="F39" s="46"/>
-      <c r="G39" s="50">
+      <c r="F45" s="59"/>
+      <c r="G45" s="15">
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="9"/>
-      <c r="B40" s="26"/>
-      <c r="C40" s="18"/>
-      <c r="D40" s="107"/>
-      <c r="E40" s="97"/>
-      <c r="F40" s="47"/>
-      <c r="G40" s="35"/>
-    </row>
-    <row r="41" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="9"/>
-      <c r="B41" s="26"/>
-      <c r="C41" s="29" t="s">
-        <v>64</v>
-      </c>
-      <c r="D41" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="E41" s="32" t="s">
-        <v>49</v>
-      </c>
-      <c r="F41" s="46"/>
-      <c r="G41" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="9"/>
-      <c r="B42" s="26"/>
-      <c r="C42" s="18"/>
-      <c r="D42" s="31"/>
-      <c r="E42" s="33"/>
-      <c r="F42" s="47"/>
-      <c r="G42" s="35"/>
-    </row>
-    <row r="43" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="9"/>
-      <c r="B43" s="26"/>
-      <c r="C43" s="29" t="s">
-        <v>72</v>
-      </c>
-      <c r="D43" s="98" t="s">
-        <v>73</v>
-      </c>
-      <c r="E43" s="100" t="s">
-        <v>74</v>
-      </c>
-      <c r="F43" s="48"/>
-      <c r="G43" s="50">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="10"/>
-      <c r="B44" s="27"/>
-      <c r="C44" s="68"/>
-      <c r="D44" s="99"/>
-      <c r="E44" s="101"/>
-      <c r="F44" s="49"/>
-      <c r="G44" s="51"/>
-    </row>
-    <row r="45" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C45" s="6"/>
-      <c r="G45" s="1"/>
-    </row>
-    <row r="46" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C46" s="6"/>
-      <c r="G46" s="1"/>
-    </row>
-    <row r="47" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="35"/>
+      <c r="B46" s="44"/>
+      <c r="C46" s="82"/>
+      <c r="D46" s="78"/>
+      <c r="E46" s="80"/>
+      <c r="F46" s="60"/>
+      <c r="G46" s="61"/>
+    </row>
+    <row r="47" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C47" s="6"/>
       <c r="G47" s="1"/>
     </row>
-    <row r="48" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C48" s="6"/>
       <c r="G48" s="1"/>
     </row>
@@ -4347,44 +4521,40 @@
       <c r="C51" s="6"/>
       <c r="G51" s="1"/>
     </row>
-    <row r="52" spans="3:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C52" s="6"/>
-      <c r="G52" s="1"/>
-    </row>
-    <row r="53" spans="3:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C53" s="6"/>
-      <c r="G53" s="1"/>
-    </row>
-    <row r="54" spans="3:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E54" s="3" t="s">
+    <row r="54" spans="3:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C54" s="6"/>
+      <c r="G54" s="1"/>
+    </row>
+    <row r="55" spans="3:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C55" s="6"/>
+      <c r="G55" s="1"/>
+    </row>
+    <row r="56" spans="3:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E56" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F54" s="5" t="s">
+      <c r="F56" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="55" spans="3:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E55" s="3" t="s">
+    <row r="57" spans="3:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E57" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F55" s="5" t="s">
+      <c r="F57" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="56" spans="3:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E56" s="4" t="s">
+    <row r="58" spans="3:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E58" s="4" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="121">
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
+  <mergeCells count="127">
     <mergeCell ref="B17:B26"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="G33:G34"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="E7:E8"/>
@@ -4393,9 +4563,9 @@
     <mergeCell ref="E13:E14"/>
     <mergeCell ref="E15:E16"/>
     <mergeCell ref="E17:E18"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="E33:E34"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="G3:G4"/>
@@ -4410,7 +4580,7 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="E43:E44"/>
     <mergeCell ref="C23:C24"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="D13:D14"/>
@@ -4420,7 +4590,7 @@
     <mergeCell ref="D21:D22"/>
     <mergeCell ref="D23:D24"/>
     <mergeCell ref="E23:E24"/>
-    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="D43:D44"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="D5:D6"/>
@@ -4442,6 +4612,8 @@
     <mergeCell ref="G9:G10"/>
     <mergeCell ref="G11:G12"/>
     <mergeCell ref="G13:G14"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="E45:E46"/>
     <mergeCell ref="F17:F18"/>
     <mergeCell ref="G17:G18"/>
     <mergeCell ref="C19:C20"/>
@@ -4458,46 +4630,54 @@
     <mergeCell ref="G19:G20"/>
     <mergeCell ref="G21:G22"/>
     <mergeCell ref="C21:C22"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="A3:A26"/>
+    <mergeCell ref="B31:B40"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="B41:B46"/>
+    <mergeCell ref="A41:A46"/>
+    <mergeCell ref="G41:G42"/>
     <mergeCell ref="F41:F42"/>
+    <mergeCell ref="E41:E42"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="D37:D38"/>
     <mergeCell ref="F43:F44"/>
+    <mergeCell ref="F45:F46"/>
+    <mergeCell ref="G43:G44"/>
+    <mergeCell ref="G45:G46"/>
+    <mergeCell ref="G35:G36"/>
     <mergeCell ref="G39:G40"/>
-    <mergeCell ref="G41:G42"/>
-    <mergeCell ref="G43:G44"/>
-    <mergeCell ref="G31:G32"/>
-    <mergeCell ref="G35:G36"/>
-    <mergeCell ref="G33:G34"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="F33:F34"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="E43:E44"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="A3:A26"/>
-    <mergeCell ref="A27:A36"/>
-    <mergeCell ref="B27:B36"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="A27:A40"/>
     <mergeCell ref="C27:C28"/>
     <mergeCell ref="D27:D28"/>
     <mergeCell ref="E27:E28"/>
     <mergeCell ref="F27:F28"/>
-    <mergeCell ref="B37:B44"/>
-    <mergeCell ref="A37:A44"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="E41:E42"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="G31:G32"/>
     <mergeCell ref="G37:G38"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="F35:F36"/>
     <mergeCell ref="F37:F38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="D33:D34"/>
     <mergeCell ref="F39:F40"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>